<commit_message>
Añadidos documentos de curso para webscrapping
</commit_message>
<xml_diff>
--- a/Coaches_carreers/Referees_support.xlsx
+++ b/Coaches_carreers/Referees_support.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\La Cima del Éxito\Futbol\Coaches_carreers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A290C06B-8406-4C46-9102-1ED607CE8A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540F9998-338B-4945-9955-4AB15FFFC03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2910" yWindow="2910" windowWidth="16875" windowHeight="10343" xr2:uid="{620CCB9D-F00A-499F-9086-805A67DF22B7}"/>
+    <workbookView minimized="1" xWindow="1028" yWindow="1028" windowWidth="22485" windowHeight="14385" firstSheet="1" activeTab="1" xr2:uid="{620CCB9D-F00A-499F-9086-805A67DF22B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="135">
   <si>
     <t>Index</t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>EdgeD%</t>
+  </si>
+  <si>
+    <t>xEdge</t>
   </si>
 </sst>
 </file>
@@ -445,7 +448,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -561,7 +564,7 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -587,6 +590,15 @@
   </cellStyles>
   <dxfs count="15">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -609,15 +621,6 @@
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -667,7 +670,7 @@
   <autoFilter ref="A1:S64" xr:uid="{31915F86-7C3D-4106-9C83-3491EFF875AF}">
     <filterColumn colId="10">
       <filters>
-        <filter val="Away"/>
+        <filter val="Draw"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -688,12 +691,12 @@
     <tableColumn id="17" xr3:uid="{371D8628-0995-4D66-88AA-359670EFA4C3}" name="Bet" totalsRowFunction="count"/>
     <tableColumn id="19" xr3:uid="{84091B38-907B-4099-88D5-22B518EDAE1E}" name="Bet2"/>
     <tableColumn id="10" xr3:uid="{39757E03-E501-40D2-B656-6712C36C0108}" name="Matches2"/>
-    <tableColumn id="11" xr3:uid="{3CA96A58-5488-46A7-B4C7-4F1C9474979C}" name="Home Team Win" totalsRowFunction="average" dataDxfId="14" totalsRowDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{16F50F65-7A95-43BD-901B-4751697CE163}" name="Draw" totalsRowFunction="average" dataDxfId="13" totalsRowDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{4C3CB33E-092F-4371-B705-BDA139B29748}" name="Away Team Win" totalsRowFunction="average" dataDxfId="12" totalsRowDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{AB78C408-596B-4057-97C7-B08E11C89DFF}" name="Home Goals Scored" dataDxfId="11" totalsRowDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{57C029B2-563E-49AA-A467-F680108DDFF1}" name="Away Scored Goals" dataDxfId="10" totalsRowDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{52453426-E459-4093-BDAE-454A1D8695E0}" name="Scored Goals Overall" dataDxfId="9" totalsRowDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{3CA96A58-5488-46A7-B4C7-4F1C9474979C}" name="Home Team Win" totalsRowFunction="average" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{16F50F65-7A95-43BD-901B-4751697CE163}" name="Draw" totalsRowFunction="average" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{4C3CB33E-092F-4371-B705-BDA139B29748}" name="Away Team Win" totalsRowFunction="average" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{AB78C408-596B-4057-97C7-B08E11C89DFF}" name="Home Goals Scored" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="15" xr3:uid="{57C029B2-563E-49AA-A467-F680108DDFF1}" name="Away Scored Goals" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{52453426-E459-4093-BDAE-454A1D8695E0}" name="Scored Goals Overall" dataDxfId="4" totalsRowDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -709,7 +712,7 @@
     <tableColumn id="20" xr3:uid="{364F3D80-8516-4CC1-BC18-3249C9BB5030}" name="hH"/>
     <tableColumn id="14" xr3:uid="{1EDEA628-618D-46E1-8810-4D15AF2C70C9}" name="hD"/>
     <tableColumn id="17" xr3:uid="{9DCDE948-7D1E-41B9-B564-485816CA8987}" name="hA"/>
-    <tableColumn id="15" xr3:uid="{5D14968E-7E0F-4D81-A4F8-A1A4670FB4F9}" name="Edge" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{5D14968E-7E0F-4D81-A4F8-A1A4670FB4F9}" name="Edge" dataDxfId="2"/>
     <tableColumn id="16" xr3:uid="{681668BE-2815-4C0C-88AA-9D4A5D8498BF}" name="H"/>
     <tableColumn id="18" xr3:uid="{5E6CD799-0CA0-43F1-A236-BE810036AC83}" name="xH"/>
     <tableColumn id="11" xr3:uid="{47E9917B-0B61-4EF6-AFDD-F86F85FDB7B9}" name="D"/>
@@ -717,13 +720,13 @@
     <tableColumn id="19" xr3:uid="{4EB34FB8-9AAA-477C-BC74-DEEFD47A2B46}" name="A"/>
     <tableColumn id="12" xr3:uid="{7DD7C757-9DB4-4B9E-A846-4E0278DE6F66}" name="xA"/>
     <tableColumn id="3" xr3:uid="{656E5EF3-5B75-43D3-A585-1F5D8B2259BA}" name="Won"/>
-    <tableColumn id="4" xr3:uid="{5219129F-A3FE-412F-8674-7671EB5C9E0C}" name="Lost" dataDxfId="7">
+    <tableColumn id="4" xr3:uid="{5219129F-A3FE-412F-8674-7671EB5C9E0C}" name="Lost" dataDxfId="1">
       <calculatedColumnFormula>Table2[[#This Row],[Matches]]-Table2[[#This Row],[Won]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{7D0F35EC-B0A3-4D56-81AB-F2F02EBBC173}" name="RatioW" dataCellStyle="Percent">
       <calculatedColumnFormula>Table2[[#This Row],[Won]]/Table2[[#This Row],[Matches]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{AF2349F3-222B-46EF-9B80-BAF00782E805}" name="Principal" dataDxfId="8">
+    <tableColumn id="6" xr3:uid="{AF2349F3-222B-46EF-9B80-BAF00782E805}" name="Principal" dataDxfId="0">
       <calculatedColumnFormula>Table2[[#This Row],[Matches]]*$C$4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{A9449722-9001-41EC-828F-74E6C4B2FF9D}" name="Earnings"/>
@@ -1033,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B510DF5-DE33-4D78-9E71-F924F93448BB}">
   <dimension ref="A1:S81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1113,7 +1116,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:19" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>71</v>
       </c>
@@ -1167,7 +1170,7 @@
         <v>-6.6638038142109561</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:19" hidden="1" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>37</v>
       </c>
@@ -1220,7 +1223,7 @@
         <v>4.8689983263079828</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>124</v>
       </c>
@@ -1274,7 +1277,7 @@
         <v>2.3142492877772147</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19" hidden="1" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1389,7 +1392,7 @@
         <v>2.8034811141943727</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>212</v>
       </c>
@@ -1504,7 +1507,7 @@
         <v>5.5392261900874429</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:19" hidden="1" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>122</v>
       </c>
@@ -1619,7 +1622,7 @@
         <v>-4.6507601321420511</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:19" hidden="1" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>180</v>
       </c>
@@ -1846,7 +1849,7 @@
         <v>7.9395525246788612</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:19" hidden="1" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>35</v>
       </c>
@@ -3480,7 +3483,7 @@
         <v>0.91295957148014306</v>
       </c>
     </row>
-    <row r="45" spans="1:19" hidden="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>193</v>
       </c>
@@ -4078,7 +4081,7 @@
         <v>-4.3964370544036342</v>
       </c>
     </row>
-    <row r="56" spans="1:19" hidden="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>280</v>
       </c>
@@ -4188,7 +4191,7 @@
         <v>-5.6567004589976104</v>
       </c>
     </row>
-    <row r="58" spans="1:19" hidden="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>103</v>
       </c>
@@ -4244,7 +4247,7 @@
         <v>-6.0106818800653716E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:19" hidden="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>8</v>
       </c>
@@ -4300,7 +4303,7 @@
         <v>0.38520617134452095</v>
       </c>
     </row>
-    <row r="60" spans="1:19" hidden="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>153</v>
       </c>
@@ -4356,7 +4359,7 @@
         <v>1.5096095047660185</v>
       </c>
     </row>
-    <row r="61" spans="1:19" hidden="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>0</v>
       </c>
@@ -4412,7 +4415,7 @@
         <v>-1.3945462688222832</v>
       </c>
     </row>
-    <row r="62" spans="1:19" hidden="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>49</v>
       </c>
@@ -4578,19 +4581,19 @@
     <row r="65" spans="10:19" x14ac:dyDescent="0.45">
       <c r="K65">
         <f>SUBTOTAL(103,Table1[Bet])</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N65" s="2">
         <f>SUBTOTAL(101,Table1[Home Team Win])</f>
-        <v>-3.3024646625561971</v>
+        <v>-5.2664751951455884</v>
       </c>
       <c r="O65" s="2">
         <f>SUBTOTAL(101,Table1[Draw])</f>
-        <v>-15.95249460060187</v>
+        <v>28.260775904395704</v>
       </c>
       <c r="P65" s="2">
         <f>SUBTOTAL(101,Table1[Away Team Win])</f>
-        <v>18.162563859759778</v>
+        <v>-17.609746361332501</v>
       </c>
       <c r="Q65" s="2"/>
       <c r="R65" s="2"/>
@@ -4856,8 +4859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8ED1CD1-D925-4B7A-A2C4-A64909981C35}">
   <dimension ref="B4:U28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5346,6 +5349,9 @@
       <c r="M21" t="s">
         <v>127</v>
       </c>
+      <c r="N21" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
@@ -5388,6 +5394,10 @@
       <c r="M22" s="1">
         <v>47.880428167892198</v>
       </c>
+      <c r="N22">
+        <f>L22/M22</f>
+        <v>1.2740069864476602</v>
+      </c>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
@@ -5430,6 +5440,10 @@
       <c r="M23" s="1">
         <v>53.137284203505899</v>
       </c>
+      <c r="N23">
+        <f>L23/M23</f>
+        <v>1.2044273801214966</v>
+      </c>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
@@ -5468,6 +5482,9 @@
       <c r="M25" t="s">
         <v>127</v>
       </c>
+      <c r="N25" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
@@ -5509,6 +5526,10 @@
       <c r="M26">
         <v>37.1</v>
       </c>
+      <c r="N26">
+        <f>J26/K26</f>
+        <v>1.1935483870967742</v>
+      </c>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
@@ -5550,6 +5571,10 @@
       <c r="M27">
         <v>62.3</v>
       </c>
+      <c r="N27">
+        <f t="shared" ref="N27:N28" si="3">J27/K27</f>
+        <v>1.2452107279693485</v>
+      </c>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
@@ -5590,6 +5615,10 @@
       </c>
       <c r="M28">
         <v>64.400000000000006</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="3"/>
+        <v>1.2979890310786106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>